<commit_message>
added new oos and tiff files
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaYGProtocol.xlsx
+++ b/Protocol/IschemiaYGProtocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="132">
   <si>
     <t>120219_P5_slc1_0003</t>
   </si>
@@ -311,20 +311,125 @@
     <t>\\IFMB-02-024B-10\Ischemia2\IOS\2019-03-29\2019-03-29_11-36-23.ios</t>
   </si>
   <si>
-    <t>300519_P17_slc1</t>
-  </si>
-  <si>
-    <t>\\IFMB-02-024B-10\Ischemia2\IOS\2019-05-30\2019-05-30_13-13-31.ios</t>
-  </si>
-  <si>
-    <t>\\IFMB-02-024B-10\Ischemia2\300519_P17_SD\300519_P17_slc1_1000.abf</t>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-03-29\2019-03-29_13-53-31.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-01\2019-04-01_10-32-46.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-01\2019-04-01_12-43-28.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-01\2019-04-01_14-29-52.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-17\2019-04-17_10-48-31.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-17\2019-04-17_13-9-59.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-04-17\2019-04-17_15-20-5.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-27\2019-05-27_13-39-7.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\270519_P8\slice1.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-27\2019-05-27_15-19-23.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\270519_P8\slice2.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-28\2019-05-28_10-19-34.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\280519_P8\slice1.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-28\2019-05-28_12-6-48.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\280519_P8\slice2.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-29\2019-05-29_13-47-36.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\290519_P8\slice1.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-29\2019-05-29_15-34-5.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\290519_P8\slice2.tif</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-05-29\2019-05-29_11-17-24.oos</t>
+  </si>
+  <si>
+    <t>\\ED02\Data_Marat\Ischemia\TTC Elvira\290519_P8\slice3.tif</t>
+  </si>
+  <si>
+    <t>290319_P3_slc4</t>
+  </si>
+  <si>
+    <t>OIS only</t>
+  </si>
+  <si>
+    <t>010419_P4_slc1</t>
+  </si>
+  <si>
+    <t>010419_P4_slc2</t>
+  </si>
+  <si>
+    <t>010419_P4_slc3</t>
+  </si>
+  <si>
+    <t>170419_P5_slc1</t>
+  </si>
+  <si>
+    <t>170419_P5_slc2</t>
+  </si>
+  <si>
+    <t>170419_P5_slc3</t>
+  </si>
+  <si>
+    <t>270519_P8_slc1</t>
+  </si>
+  <si>
+    <t>270519_P8_slc2</t>
+  </si>
+  <si>
+    <t>280519_P8_slc1</t>
+  </si>
+  <si>
+    <t>280519_P8_slc2</t>
+  </si>
+  <si>
+    <t>290519_P8_slc1</t>
+  </si>
+  <si>
+    <t>290519_P8_slc2</t>
+  </si>
+  <si>
+    <t>290519_P8_slc3</t>
+  </si>
+  <si>
+    <t>TTC tiff file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,8 +453,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,8 +490,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -421,6 +544,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -428,7 +571,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,6 +623,52 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -488,7 +677,31 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Примечание" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -565,8 +778,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -581,24 +794,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:O26" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O26"/>
-  <tableColumns count="15">
-    <tableColumn id="12" name="ID" dataDxfId="14"/>
-    <tableColumn id="1" name="name" dataDxfId="13"/>
-    <tableColumn id="2" name="age" dataDxfId="12"/>
-    <tableColumn id="3" name="type\comment" dataDxfId="11"/>
-    <tableColumn id="4" name="ABF file" dataDxfId="10" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="5" name="IOS file" dataDxfId="9"/>
-    <tableColumn id="6" name="AD" dataDxfId="8"/>
-    <tableColumn id="7" name="SD" dataDxfId="7"/>
-    <tableColumn id="8" name="OGD time" dataDxfId="6"/>
-    <tableColumn id="9" name="wash time" dataDxfId="5"/>
-    <tableColumn id="10" name="AD time" dataDxfId="4"/>
-    <tableColumn id="11" name="SD time" dataDxfId="3"/>
-    <tableColumn id="13" name="CDS" dataDxfId="2"/>
-    <tableColumn id="14" name="LSS" dataDxfId="1"/>
-    <tableColumn id="15" name="synchronized steps and stimuli" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:P39" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P39"/>
+  <tableColumns count="16">
+    <tableColumn id="12" name="ID" dataDxfId="15"/>
+    <tableColumn id="1" name="name" dataDxfId="14"/>
+    <tableColumn id="2" name="age" dataDxfId="13"/>
+    <tableColumn id="3" name="type\comment" dataDxfId="12"/>
+    <tableColumn id="4" name="ABF file" dataDxfId="11" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="5" name="IOS file" dataDxfId="10"/>
+    <tableColumn id="16" name="TTC tiff file" dataDxfId="0"/>
+    <tableColumn id="6" name="AD" dataDxfId="9"/>
+    <tableColumn id="7" name="SD" dataDxfId="8"/>
+    <tableColumn id="8" name="OGD time" dataDxfId="7"/>
+    <tableColumn id="9" name="wash time" dataDxfId="6"/>
+    <tableColumn id="10" name="AD time" dataDxfId="5"/>
+    <tableColumn id="11" name="SD time" dataDxfId="4"/>
+    <tableColumn id="13" name="CDS" dataDxfId="3"/>
+    <tableColumn id="14" name="LSS" dataDxfId="2"/>
+    <tableColumn id="15" name="synchronized steps and stimuli" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -867,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,20 +1094,20 @@
     <col min="3" max="3" width="5.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="26.88671875" style="6" customWidth="1"/>
     <col min="5" max="5" width="22.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="6"/>
-    <col min="8" max="8" width="10.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.44140625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" style="6" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="6"/>
+    <col min="6" max="7" width="14.109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="10.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.21875" style="6" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.44140625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="18.44140625" style="6" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>65</v>
       </c>
@@ -913,34 +1127,37 @@
         <v>59</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>446</v>
       </c>
@@ -959,29 +1176,30 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="6">
         <v>0</v>
       </c>
       <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
         <v>10.1341866666667</v>
       </c>
-      <c r="J2" s="6">
+      <c r="K2" s="6">
         <v>36.997120000000002</v>
       </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
       <c r="N2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>447</v>
       </c>
@@ -1000,32 +1218,33 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="6">
         <v>1</v>
       </c>
       <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
         <v>5.3683199999999998</v>
       </c>
-      <c r="J3" s="6">
+      <c r="K3" s="6">
         <v>32.178346666666698</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>32.4</v>
       </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
       <c r="N3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>450</v>
       </c>
@@ -1044,32 +1263,33 @@
       <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="6">
         <v>1</v>
       </c>
       <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6">
         <v>5.3546666666666702</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>27.054079999999999</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>27.1635574416667</v>
       </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
       <c r="N4" s="6">
         <v>1</v>
       </c>
       <c r="O4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>451</v>
       </c>
@@ -1088,32 +1308,33 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="14">
-        <v>1</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="14">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
         <v>5.0713600000000003</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
         <v>37.668693333333302</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <v>21.41</v>
       </c>
-      <c r="M5" s="6">
-        <v>1</v>
-      </c>
       <c r="N5" s="6">
         <v>1</v>
       </c>
       <c r="O5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>452</v>
       </c>
@@ -1132,32 +1353,33 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="6">
         <v>1</v>
       </c>
       <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
         <v>5.9272533333333302</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="6">
         <v>30.330026666666701</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>30.6631568666667</v>
       </c>
-      <c r="M6" s="6">
-        <v>1</v>
-      </c>
       <c r="N6" s="6">
         <v>1</v>
       </c>
       <c r="O6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>453</v>
       </c>
@@ -1176,29 +1398,30 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="14">
-        <v>1</v>
-      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="14">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
+      <c r="J7" s="6">
         <v>4.7419733333333296</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="6">
         <v>36.912640000000003</v>
       </c>
-      <c r="M7" s="6">
-        <v>1</v>
-      </c>
       <c r="N7" s="6">
         <v>1</v>
       </c>
       <c r="O7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>454</v>
       </c>
@@ -1217,32 +1440,33 @@
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="6">
         <v>1</v>
       </c>
       <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
         <v>4.8861866666666698</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="6">
         <v>42.554879999999997</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>42.411812079166701</v>
       </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
       <c r="N8" s="6">
         <v>1</v>
       </c>
       <c r="O8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>455</v>
       </c>
@@ -1261,32 +1485,33 @@
       <c r="F9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="14">
-        <v>0</v>
-      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="14">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
         <v>5.0662399999999996</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="6">
         <v>48.138240000000003</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <v>48.744420562499997</v>
       </c>
-      <c r="M9" s="6">
-        <v>1</v>
-      </c>
       <c r="N9" s="6">
         <v>1</v>
       </c>
       <c r="O9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>456</v>
       </c>
@@ -1305,32 +1530,33 @@
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="6">
-        <v>1</v>
-      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="6">
         <v>1</v>
       </c>
       <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
         <v>4.8887466666666697</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="6">
         <v>16.052053333333301</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <v>16.3314639833333</v>
       </c>
-      <c r="M10" s="6">
-        <v>1</v>
-      </c>
       <c r="N10" s="6">
         <v>1</v>
       </c>
       <c r="O10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>457</v>
       </c>
@@ -1349,32 +1575,33 @@
       <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="14">
-        <v>0</v>
-      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="14">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
         <v>5.5748266666666701</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="6">
         <v>21.175466666666701</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="6">
         <v>20.830948958333298</v>
       </c>
-      <c r="M11" s="6">
-        <v>1</v>
-      </c>
       <c r="N11" s="6">
         <v>1</v>
       </c>
       <c r="O11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>458</v>
       </c>
@@ -1393,32 +1620,33 @@
       <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="6">
         <v>1</v>
       </c>
       <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
         <v>5.3700266666666696</v>
       </c>
-      <c r="J12" s="6">
+      <c r="K12" s="6">
         <v>19.277653333333301</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="6">
         <v>19.331120633333299</v>
       </c>
-      <c r="M12" s="6">
-        <v>1</v>
-      </c>
       <c r="N12" s="6">
         <v>1</v>
       </c>
       <c r="O12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>459</v>
       </c>
@@ -1437,32 +1665,33 @@
       <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="6">
-        <v>1</v>
-      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="6">
         <v>1</v>
       </c>
       <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
         <v>5.2147199999999998</v>
       </c>
-      <c r="J13" s="6">
+      <c r="K13" s="6">
         <v>35.636906666666697</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <v>22.164129691666702</v>
       </c>
-      <c r="M13" s="6">
-        <v>1</v>
-      </c>
       <c r="N13" s="6">
         <v>1</v>
       </c>
       <c r="O13" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>460</v>
       </c>
@@ -1481,32 +1710,33 @@
       <c r="F14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="6">
-        <v>1</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="6">
         <v>1</v>
       </c>
       <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
         <v>10.128213333333299</v>
       </c>
-      <c r="J14" s="6">
+      <c r="K14" s="6">
         <v>25.046186666666699</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <v>25.413757729166701</v>
       </c>
-      <c r="M14" s="6">
-        <v>1</v>
-      </c>
       <c r="N14" s="6">
         <v>1</v>
       </c>
       <c r="O14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>461</v>
       </c>
@@ -1525,32 +1755,33 @@
       <c r="F15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="6">
-        <v>1</v>
-      </c>
+      <c r="G15" s="1"/>
       <c r="H15" s="6">
         <v>1</v>
       </c>
       <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
         <v>5.1413333333333302</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>18.133333333333301</v>
       </c>
-      <c r="L15" s="6">
+      <c r="M15" s="6">
         <v>18.247911287499999</v>
       </c>
-      <c r="M15" s="6">
-        <v>1</v>
-      </c>
       <c r="N15" s="6">
         <v>1</v>
       </c>
       <c r="O15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>462</v>
       </c>
@@ -1569,32 +1800,33 @@
       <c r="F16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="6">
-        <v>1</v>
-      </c>
+      <c r="G16" s="1"/>
       <c r="H16" s="6">
         <v>1</v>
       </c>
       <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
         <v>5.2915200000000002</v>
       </c>
-      <c r="J16" s="6">
+      <c r="K16" s="6">
         <v>20.0149333333333</v>
       </c>
-      <c r="L16" s="6">
+      <c r="M16" s="6">
         <v>20.164358591666701</v>
       </c>
-      <c r="M16" s="6">
-        <v>1</v>
-      </c>
       <c r="N16" s="6">
         <v>1</v>
       </c>
       <c r="O16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>468</v>
       </c>
@@ -1613,29 +1845,30 @@
       <c r="F17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="6">
-        <v>1</v>
-      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="6">
         <v>1</v>
       </c>
       <c r="I17" s="6">
+        <v>1</v>
+      </c>
+      <c r="J17" s="6">
         <v>12.70528</v>
       </c>
-      <c r="J17" s="6">
+      <c r="K17" s="6">
         <v>70.737066666666706</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="6">
         <v>56.66</v>
       </c>
-      <c r="N17" s="6">
-        <v>1</v>
-      </c>
       <c r="O17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>469</v>
       </c>
@@ -1654,26 +1887,27 @@
       <c r="F18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="1"/>
+      <c r="H18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="6">
-        <v>1</v>
-      </c>
       <c r="I18" s="6">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6">
         <v>5.8786133333333304</v>
       </c>
-      <c r="J18" s="6">
+      <c r="K18" s="6">
         <v>47.435093333333299</v>
       </c>
-      <c r="L18" s="6">
+      <c r="M18" s="6">
         <v>40.299999999999997</v>
       </c>
-      <c r="O18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>470</v>
       </c>
@@ -1692,26 +1926,27 @@
       <c r="F19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="1"/>
+      <c r="H19" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H19" s="6">
-        <v>1</v>
-      </c>
       <c r="I19" s="6">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
         <v>8.8644266666666702</v>
       </c>
-      <c r="J19" s="6">
+      <c r="K19" s="6">
         <v>62.879573333333298</v>
       </c>
-      <c r="L19" s="6">
+      <c r="M19" s="6">
         <v>55</v>
       </c>
-      <c r="O19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>471</v>
       </c>
@@ -1730,23 +1965,24 @@
       <c r="F20" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="11"/>
+      <c r="H20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H20" s="6">
-        <v>1</v>
-      </c>
       <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
         <v>5.6311467000000004</v>
       </c>
-      <c r="J20" s="6">
+      <c r="K20" s="6">
         <v>42.317653300000003</v>
       </c>
-      <c r="L20" s="6">
+      <c r="M20" s="6">
         <v>28.5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>472</v>
       </c>
@@ -1763,8 +1999,9 @@
       <c r="F21" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>473</v>
       </c>
@@ -1781,8 +2018,9 @@
       <c r="F22" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>474</v>
       </c>
@@ -1799,8 +2037,9 @@
       <c r="F23" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>475</v>
       </c>
@@ -1817,8 +2056,9 @@
       <c r="F24" s="11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>476</v>
       </c>
@@ -1835,22 +2075,293 @@
       <c r="F25" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
-        <v>491</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="27">
+        <v>477</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="29">
+        <v>3</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="11">
-        <v>17</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="27">
+        <v>478</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="29">
+        <v>4</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="27">
+        <v>479</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="29">
+        <v>4</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>96</v>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="27">
+        <v>480</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="27">
+        <v>481</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="29">
+        <v>5</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="27">
+        <v>482</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="29">
+        <v>5</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="27">
+        <v>483</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="29">
+        <v>5</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="12"/>
+      <c r="F32" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="27">
+        <v>484</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="32">
+        <v>8</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="27">
+        <v>485</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="32">
+        <v>8</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="27">
+        <v>486</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="32">
+        <v>8</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="27">
+        <v>487</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="32">
+        <v>8</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="27">
+        <v>488</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="32">
+        <v>8</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="27">
+        <v>489</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="32">
+        <v>8</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="27">
+        <v>490</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="32">
+        <v>8</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1875,10 +2386,13 @@
     <hyperlink ref="E16" r:id="rId18"/>
     <hyperlink ref="E20" r:id="rId19"/>
     <hyperlink ref="F22" r:id="rId20"/>
+    <hyperlink ref="G33" r:id="rId21"/>
+    <hyperlink ref="G35" r:id="rId22"/>
+    <hyperlink ref="G36" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
scrips for OIS video, traces and other things with my .oos files
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaYGProtocol.xlsx
+++ b/Protocol/IschemiaYGProtocol.xlsx
@@ -571,7 +571,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,6 +669,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1084,7 +1087,7 @@
   <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2171,7 +2174,7 @@
         <v>117</v>
       </c>
       <c r="E30" s="12"/>
-      <c r="F30" s="18" t="s">
+      <c r="F30" s="34" t="s">
         <v>99</v>
       </c>
       <c r="G30" s="18"/>
@@ -2389,10 +2392,11 @@
     <hyperlink ref="G33" r:id="rId21"/>
     <hyperlink ref="G35" r:id="rId22"/>
     <hyperlink ref="G36" r:id="rId23"/>
+    <hyperlink ref="F30" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes and common analysis
</commit_message>
<xml_diff>
--- a/Protocol/IschemiaYGProtocol.xlsx
+++ b/Protocol/IschemiaYGProtocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="160">
   <si>
     <t>120219_P5_slc1_0003</t>
   </si>
@@ -281,9 +281,6 @@
     <t>210319_P3_pair1</t>
   </si>
   <si>
-    <t>210319_P3_pair2</t>
-  </si>
-  <si>
     <t>two slices, only IOS</t>
   </si>
   <si>
@@ -420,6 +417,93 @@
   </si>
   <si>
     <t>TTC tiff file</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\110719_P6\110719_P6_slice 1_1000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-07-11\2019-07-11_13-5-36.oos</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\120719_P7\120719_P7_slic 2_cell7_1000.abf</t>
+  </si>
+  <si>
+    <t>120719_P7_OGD</t>
+  </si>
+  <si>
+    <t>110719_P6_OGD</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\OOS\2019-07-12\2019-07-12_11-57-51.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-07-16\2019-07-16_10-30-23.oos</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\160719_P4\160719_P4_slc1_cell7_EXP_1000.abf</t>
+  </si>
+  <si>
+    <t>160719_P4_slc1</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\110719_P6_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\120719_P7_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\160719_P4_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>OIS в L4</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\170719_P17_slc1_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>170719_P17_OGD</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-07-17\2019-07-17_11-22-2.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\170719_P17\170719_P17_slc1_CONTROL_cell6_1000.abf</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\180719_P5\180719_P5_slc1_EXP_cell8_1000.abf</t>
+  </si>
+  <si>
+    <t>180719_P5_OGD</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\180719_P5_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\OOS\2019-07-18\2019-07-18_12-33-49.oos</t>
+  </si>
+  <si>
+    <t>190719_P5_OGD</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\190719_P5\190719_P5_slc1_EXP_cell7_1000.abf</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\OOS\2019-07-19\2019-07-19_11-28-14.oos</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\190719_P5_OGD.xlsx</t>
+  </si>
+  <si>
+    <t>\\ifmb-02-024b-10\Ischemia2\OOS\2019-07-22\2019-07-22_13-42-55.oos</t>
+  </si>
+  <si>
+    <t>\\IFMB-02-024B-10\Ischemia2\220719_P16\220719_P16_slc1_EXP_cell7_1000.abf</t>
+  </si>
+  <si>
+    <t>220719_P16_OGD</t>
+  </si>
+  <si>
+    <t>D:\Neurolab\ialdev\Ischemia YG\Protocol\220719_P16_OGD.xlsx</t>
   </si>
 </sst>
 </file>
@@ -429,7 +513,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +541,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -571,7 +663,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,6 +764,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -797,8 +899,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:P39" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:P45" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P45"/>
   <tableColumns count="16">
     <tableColumn id="12" name="ID" dataDxfId="15"/>
     <tableColumn id="1" name="name" dataDxfId="14"/>
@@ -1084,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1103,7 +1205,7 @@
     <col min="10" max="10" width="11.21875" style="6" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" style="6" customWidth="1"/>
     <col min="12" max="12" width="10.44140625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" style="6" customWidth="1"/>
     <col min="14" max="14" width="8.44140625" style="6" customWidth="1"/>
     <col min="15" max="15" width="8.6640625" style="6" customWidth="1"/>
     <col min="16" max="16" width="18.44140625" style="6" customWidth="1"/>
@@ -1130,7 +1232,7 @@
         <v>59</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>62</v>
@@ -1154,7 +1256,7 @@
         <v>80</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>69</v>
@@ -1996,7 +2098,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="11" t="s">
@@ -2009,13 +2111,13 @@
         <v>473</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="C22" s="11">
         <v>3</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
@@ -2028,17 +2130,17 @@
         <v>474</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="11">
         <v>3</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="11"/>
     </row>
@@ -2047,17 +2149,17 @@
         <v>475</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="11">
         <v>3</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G24" s="11"/>
     </row>
@@ -2066,17 +2168,17 @@
         <v>476</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="11">
         <v>3</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" s="11"/>
     </row>
@@ -2085,17 +2187,17 @@
         <v>477</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="29">
         <v>3</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="19"/>
@@ -2105,17 +2207,17 @@
         <v>478</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="29">
         <v>4</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="19"/>
@@ -2125,17 +2227,17 @@
         <v>479</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" s="29">
         <v>4</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="19"/>
@@ -2145,17 +2247,17 @@
         <v>480</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="29">
         <v>4</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="19"/>
@@ -2165,17 +2267,17 @@
         <v>481</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="29">
         <v>5</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="19"/>
@@ -2185,17 +2287,17 @@
         <v>482</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="29">
         <v>5</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="19"/>
@@ -2205,166 +2307,324 @@
         <v>483</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="29">
         <v>5</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="19"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="27">
         <v>484</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="32">
         <v>8</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="27">
         <v>485</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="32">
         <v>8</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G34" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="27">
         <v>486</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="32">
         <v>8</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G35" s="23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="27">
         <v>487</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C36" s="32">
         <v>8</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="G36" s="24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="27">
         <v>488</v>
       </c>
       <c r="B37" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" s="32">
         <v>8</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G37" s="25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="27">
         <v>489</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C38" s="32">
         <v>8</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E38" s="12"/>
       <c r="F38" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="27">
         <v>490</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="32">
         <v>8</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="11">
+        <v>526</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="11">
+        <v>6</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G40" s="22"/>
+      <c r="O40" s="6">
+        <v>0</v>
+      </c>
+      <c r="P40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="11">
+        <v>549</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="11">
+        <v>7</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" s="22"/>
+      <c r="O41" s="6">
+        <v>1</v>
+      </c>
+      <c r="P41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
+        <v>551</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="11">
+        <v>4</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="22"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="11">
+        <v>552</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="36">
+        <v>17</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="G43" s="22"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="11">
+        <v>553</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="11">
+        <v>5</v>
+      </c>
+      <c r="D44" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="11">
+        <v>554</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="11">
+        <v>5</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="22"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>555</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="38">
+        <v>16</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2393,10 +2653,23 @@
     <hyperlink ref="G35" r:id="rId22"/>
     <hyperlink ref="G36" r:id="rId23"/>
     <hyperlink ref="F30" r:id="rId24"/>
+    <hyperlink ref="D40" r:id="rId25"/>
+    <hyperlink ref="D41" r:id="rId26"/>
+    <hyperlink ref="D42" r:id="rId27"/>
+    <hyperlink ref="E40" r:id="rId28"/>
+    <hyperlink ref="E41" r:id="rId29"/>
+    <hyperlink ref="E42" r:id="rId30"/>
+    <hyperlink ref="E43" r:id="rId31"/>
+    <hyperlink ref="D44" r:id="rId32"/>
+    <hyperlink ref="D45" r:id="rId33" display="&quot;D:\Neurolab\ialdev\Ischemia YG\Protocol\190719_P5_OGD.xlsx&quot;"/>
+    <hyperlink ref="D43" r:id="rId34"/>
+    <hyperlink ref="E46" r:id="rId35"/>
+    <hyperlink ref="D46" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
   <tableParts count="1">
-    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId38"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>